<commit_message>
French Concessive Analysis Added french_analysis.R has been updated for the concessive data.
</commit_message>
<xml_diff>
--- a/spr_task/allwords_split.xlsx
+++ b/spr_task/allwords_split.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herts\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herts\OneDrive\Desktop\Manu\connectives\spr_task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13291054-4E0F-4936-9011-FBAD52821279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ABE27E-0ED5-4D61-89A2-704C72F9322F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="30" windowWidth="19160" windowHeight="10020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="180" windowWidth="19190" windowHeight="10020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="allwords" sheetId="1" r:id="rId1"/>
@@ -7571,12 +7571,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -18500,7 +18499,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H183" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C383" workbookViewId="0">
       <selection activeCell="P190" sqref="P190"/>
     </sheetView>
   </sheetViews>
@@ -35240,7 +35239,7 @@
       <c r="W188" s="1" t="s">
         <v>1338</v>
       </c>
-      <c r="X188" s="4" t="s">
+      <c r="X188" t="s">
         <v>975</v>
       </c>
       <c r="Y188" s="2" t="s">

</xml_diff>